<commit_message>
add readme and some other small updates
</commit_message>
<xml_diff>
--- a/data_scripts/scripts/GraphTextV2.xlsx
+++ b/data_scripts/scripts/GraphTextV2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10F211C-D91F-4D4D-90FA-4C777D0BD13B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D91C14-25EC-A945-8410-D3B19BF7BE3A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28000" yWindow="-6180" windowWidth="25600" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dan_6_21" sheetId="2" r:id="rId1"/>
@@ -2978,9 +2978,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="29">
+  <fonts count="30">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -3213,126 +3220,127 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3725,10 +3733,10 @@
   <dimension ref="A1:AQ255"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomRight" activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -6873,7 +6881,7 @@
       <c r="F41" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="G41" s="43" t="s">
+      <c r="G41" s="82" t="s">
         <v>573</v>
       </c>
       <c r="H41" s="8"/>

</xml_diff>